<commit_message>
Added: - feature transformation - missing values imputation
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7360" yWindow="460" windowWidth="28800" windowHeight="19500" tabRatio="500"/>
+    <workbookView xWindow="180" yWindow="520" windowWidth="25720" windowHeight="19500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">metadata!$A$1:$G$49</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="166">
   <si>
     <t>name</t>
   </si>
@@ -486,6 +486,48 @@
   </si>
   <si>
     <t>datetime</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>dummy</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t>nan_share</t>
+  </si>
+  <si>
+    <t>drop</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>encode</t>
+  </si>
+  <si>
+    <t>X49</t>
+  </si>
+  <si>
+    <t>month_action</t>
+  </si>
+  <si>
+    <t>X50</t>
+  </si>
+  <si>
+    <t>month_joined</t>
+  </si>
+  <si>
+    <t>Created based on the DateTimeIndex of X1</t>
+  </si>
+  <si>
+    <t>Created based on the DateTimeIndex of X7</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
@@ -528,10 +570,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,15 +602,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>323273</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>184727</xdr:rowOff>
+      <xdr:colOff>531091</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>80818</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3679537</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>184727</xdr:rowOff>
+      <xdr:colOff>3887355</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>80817</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -568,8 +619,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="323273" y="10367818"/>
-          <a:ext cx="4603173" cy="2078182"/>
+          <a:off x="1570182" y="12700000"/>
+          <a:ext cx="4603173" cy="2078181"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -972,716 +1023,1122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:H68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="69" style="3" customWidth="1"/>
+    <col min="4" max="5" width="11.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>102</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>103</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>105</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>106</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>107</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>152</v>
+      </c>
+      <c r="H6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>108</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>109</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" t="s">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>110</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>152</v>
+      </c>
+      <c r="H9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>112</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>113</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="2">
+        <v>0.99819999999999998</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>114</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>115</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>116</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>152</v>
+      </c>
+      <c r="H15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>117</v>
       </c>
       <c r="B16" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H16" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>118</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>119</v>
       </c>
       <c r="B18" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>120</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>152</v>
+      </c>
+      <c r="H19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>121</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F20" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>122</v>
       </c>
       <c r="B21" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>123</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="2"/>
+      <c r="E22" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>124</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>125</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>126</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G25" t="s">
+        <v>152</v>
+      </c>
+      <c r="H25" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>127</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>152</v>
+      </c>
+      <c r="H26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>128</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>152</v>
+      </c>
+      <c r="H27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>129</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>152</v>
+      </c>
+      <c r="H28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>130</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>152</v>
+      </c>
+      <c r="H29" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>131</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>152</v>
+      </c>
+      <c r="H30" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>132</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D31" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>152</v>
+      </c>
+      <c r="H31" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>133</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>152</v>
+      </c>
+      <c r="H32" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>134</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="D33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>152</v>
+      </c>
+      <c r="H33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>135</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C34" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="D34" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>152</v>
+      </c>
+      <c r="H34" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>136</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" t="s">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>152</v>
+      </c>
+      <c r="H35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>137</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>152</v>
+      </c>
+      <c r="H36" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>138</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C37" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="D37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>152</v>
+      </c>
+      <c r="H37" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>139</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C38" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D38" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>152</v>
+      </c>
+      <c r="H38" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>140</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C39" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="D39" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>152</v>
+      </c>
+      <c r="H39" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>141</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D40" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" t="s">
+        <v>152</v>
+      </c>
+      <c r="H40" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>142</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="C41" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" t="s">
+        <v>5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>152</v>
+      </c>
+      <c r="H41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>143</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D42" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" t="s">
+        <v>5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>152</v>
+      </c>
+      <c r="H42" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>144</v>
       </c>
       <c r="B43" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D43" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>152</v>
+      </c>
+      <c r="H43" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>145</v>
       </c>
       <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>152</v>
+      </c>
+      <c r="H44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>146</v>
       </c>
       <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D45" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>152</v>
+      </c>
+      <c r="H45" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>147</v>
       </c>
       <c r="B46" t="s">
         <v>49</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="D46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>152</v>
+      </c>
+      <c r="H46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>148</v>
       </c>
       <c r="B47" t="s">
         <v>50</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G47" t="s">
+        <v>152</v>
+      </c>
+      <c r="H47" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>149</v>
       </c>
       <c r="B48" t="s">
         <v>51</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G48" t="s">
+        <v>152</v>
+      </c>
+      <c r="H48" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>150</v>
       </c>
       <c r="B49" t="s">
         <v>52</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D49" t="s">
-        <v>5</v>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>152</v>
+      </c>
+      <c r="H49" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>159</v>
+      </c>
+      <c r="B50" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="66" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E66" s="1">
+        <v>110</v>
+      </c>
+      <c r="F66">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E67" s="1">
+        <v>117</v>
+      </c>
+      <c r="F67">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="68" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E68" s="1">
+        <f>110/117</f>
+        <v>0.94017094017094016</v>
+      </c>
+      <c r="F68">
+        <f>90/92-E68</f>
+        <v>3.8089929394277244E-2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1"/>
+  <autoFilter ref="A1:G49"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>